<commit_message>
Migrated all SAP services to use external ERP service
</commit_message>
<xml_diff>
--- a/src/test/data/contracts-import.xlsx
+++ b/src/test/data/contracts-import.xlsx
@@ -13,14 +13,14 @@
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
-      <loext:extCalcPr stringRefSyntax="CalcA1"/>
+      <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="14">
   <si>
     <t xml:space="preserve">Viljelijän SAP-tunnus</t>
   </si>
@@ -34,6 +34,9 @@
     <t xml:space="preserve">määrän kommentti</t>
   </si>
   <si>
+    <t xml:space="preserve">100</t>
+  </si>
+  <si>
     <t xml:space="preserve">Toimituspaikan SAP-tunnus</t>
   </si>
   <si>
@@ -43,7 +46,10 @@
     <t xml:space="preserve">SAP-kommentti</t>
   </si>
   <si>
-    <t xml:space="preserve">tusap1</t>
+    <t xml:space="preserve">111111</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1234</t>
   </si>
   <si>
     <t xml:space="preserve">Test comment</t>
@@ -62,14 +68,14 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
+  <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="@"/>
   </numFmts>
   <fonts count="4">
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
@@ -136,7 +142,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -160,81 +166,70 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
+      <selection pane="topLeft" activeCell="C3" activeCellId="0" sqref="C3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
-  <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="19.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.23"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="14.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="21.67"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="0" width="16.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="25.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="22.79"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="13.63"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1024" min="1024" style="0" width="11.52"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="8.50390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="0" t="s">
+      <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="0" t="s">
+      <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="0" t="s">
+      <c r="C1" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="0" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="n">
-        <v>100</v>
-      </c>
-      <c r="F1" s="0" t="s">
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="0" t="s">
+      <c r="F1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="H1" s="0" t="s">
+      <c r="G1" s="1" t="s">
         <v>6</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>7</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B2" s="0" t="n">
-        <v>1234</v>
-      </c>
-      <c r="C2" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" s="1" t="n">
         <v>10000</v>
       </c>
-      <c r="D2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="E2" s="0" t="s">
-        <v>9</v>
+      <c r="D2" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="E2" s="1" t="s">
+        <v>11</v>
       </c>
       <c r="F2" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G2" s="0" t="s">
-        <v>8</v>
-      </c>
-      <c r="H2" s="0" t="s">
-        <v>11</v>
+      <c r="H2" s="1" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511811023622047" footer="0.511811023622047"/>
+  <pageSetup paperSize="9" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
-    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
-    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+    <oddHeader/>
+    <oddFooter/>
   </headerFooter>
 </worksheet>
 </file>
</xml_diff>